<commit_message>
Revised Stats, 1.7 and 1.8 Ghanam - 02/03/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.3 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACAAF87D-410B-45D8-847D-B50C9677313D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4296F91-9A37-4FA6-B8C2-FF68BB5F504D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4717,10 +4717,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1577"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A355" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="N362" sqref="N362"/>
+      <selection pane="bottomLeft" activeCell="Q1510" sqref="Q1510"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
nmv 12 11 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.3 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFD3365-04CE-4D99-BD0F-453639E8C342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D28D0B5-A633-4CDE-AC01-41E77F5ED7AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4275" uniqueCount="1331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4275" uniqueCount="1330">
   <si>
     <t>PS</t>
   </si>
@@ -3567,9 +3567,6 @@
   </si>
   <si>
     <t xml:space="preserve">Asthi#taqmityA - sthiqtaqm </t>
-  </si>
-  <si>
-    <t xml:space="preserve">oSha#dhIByaq ityoShA#dhi - ByaqH </t>
   </si>
   <si>
     <t xml:space="preserve">aho$ByAqmityaha#H - ByAqm </t>
@@ -4282,7 +4279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4455,6 +4452,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -4739,10 +4739,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1568"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A617" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A815" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="V625" sqref="V625"/>
+      <selection pane="bottomLeft" activeCell="N816" sqref="N816"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -5214,7 +5214,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="72" x14ac:dyDescent="0.25">
       <c r="A1" s="50" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15" t="s">
@@ -5266,10 +5266,10 @@
         <v>10</v>
       </c>
       <c r="S1" s="39" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="T1" s="39" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="U1" s="38" t="s">
         <v>17</v>
@@ -5420,7 +5420,7 @@
         <v>4</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>0</v>
@@ -13100,7 +13100,7 @@
     </row>
     <row r="264" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A264" s="51" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="H264" s="47" t="s">
         <v>138</v>
@@ -13130,7 +13130,7 @@
     </row>
     <row r="265" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A265" s="51" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="H265" s="47" t="s">
         <v>138</v>
@@ -13629,7 +13629,7 @@
     </row>
     <row r="284" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A284" s="51" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="H284" s="47" t="s">
         <v>139</v>
@@ -13664,7 +13664,7 @@
     </row>
     <row r="285" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A285" s="51" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="H285" s="47" t="s">
         <v>139</v>
@@ -13919,7 +13919,7 @@
     </row>
     <row r="295" spans="4:22" x14ac:dyDescent="0.25">
       <c r="F295" s="54" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="I295" s="8" t="s">
         <v>23</v>
@@ -13946,7 +13946,7 @@
     </row>
     <row r="296" spans="4:22" x14ac:dyDescent="0.25">
       <c r="F296" s="54" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="I296" s="8" t="s">
         <v>23</v>
@@ -13977,7 +13977,7 @@
         <v>128</v>
       </c>
       <c r="F297" s="54" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="I297" s="8" t="s">
         <v>23</v>
@@ -14007,7 +14007,7 @@
     </row>
     <row r="298" spans="4:22" x14ac:dyDescent="0.25">
       <c r="F298" s="54" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="I298" s="8" t="s">
         <v>23</v>
@@ -15829,7 +15829,7 @@
     </row>
     <row r="368" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D368" s="48" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="H368" s="47" t="s">
         <v>141</v>
@@ -20366,7 +20366,7 @@
         <v>83</v>
       </c>
       <c r="V544" s="59" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="545" spans="9:22" x14ac:dyDescent="0.25">
@@ -22420,7 +22420,7 @@
         <v>96</v>
       </c>
       <c r="V625" s="59" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="626" spans="1:22" x14ac:dyDescent="0.25">
@@ -23112,10 +23112,10 @@
     </row>
     <row r="652" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E652" s="54" t="s">
+        <v>1315</v>
+      </c>
+      <c r="F652" s="54" t="s">
         <v>1316</v>
-      </c>
-      <c r="F652" s="54" t="s">
-        <v>1317</v>
       </c>
       <c r="I652" s="8" t="s">
         <v>30</v>
@@ -23142,10 +23142,10 @@
     </row>
     <row r="653" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E653" s="54" t="s">
+        <v>1315</v>
+      </c>
+      <c r="F653" s="54" t="s">
         <v>1316</v>
-      </c>
-      <c r="F653" s="54" t="s">
-        <v>1317</v>
       </c>
       <c r="I653" s="8" t="s">
         <v>30</v>
@@ -23383,7 +23383,7 @@
         <v>83</v>
       </c>
       <c r="V661" s="57" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="662" spans="8:22" x14ac:dyDescent="0.25">
@@ -24705,7 +24705,7 @@
     </row>
     <row r="713" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E713" s="54" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="H713" s="47" t="s">
         <v>147</v>
@@ -24743,7 +24743,7 @@
     </row>
     <row r="714" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E714" s="54" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="H714" s="47" t="s">
         <v>147</v>
@@ -24781,7 +24781,7 @@
     </row>
     <row r="715" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E715" s="54" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="H715" s="47" t="s">
         <v>147</v>
@@ -24814,7 +24814,7 @@
     </row>
     <row r="716" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E716" s="54" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="H716" s="47" t="s">
         <v>147</v>
@@ -27410,8 +27410,8 @@
       <c r="O816" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="V816" s="32" t="s">
-        <v>1177</v>
+      <c r="V816" s="60" t="s">
+        <v>1141</v>
       </c>
     </row>
     <row r="817" spans="9:22" x14ac:dyDescent="0.25">
@@ -27514,7 +27514,7 @@
         <v>0</v>
       </c>
       <c r="V820" s="14" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="821" spans="9:22" x14ac:dyDescent="0.25">
@@ -28696,7 +28696,7 @@
         <v>0</v>
       </c>
       <c r="V867" s="14" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="868" spans="8:22" x14ac:dyDescent="0.25">
@@ -28749,7 +28749,7 @@
         <v>83</v>
       </c>
       <c r="V869" s="35" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="870" spans="8:22" x14ac:dyDescent="0.25">
@@ -28903,7 +28903,7 @@
         <v>0</v>
       </c>
       <c r="V875" s="14" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="876" spans="8:22" x14ac:dyDescent="0.25">
@@ -29027,13 +29027,13 @@
         <v>11</v>
       </c>
       <c r="N880" s="5" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="O880" s="2" t="s">
         <v>0</v>
       </c>
       <c r="V880" s="14" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="881" spans="4:22" x14ac:dyDescent="0.25">
@@ -29145,7 +29145,7 @@
         <v>105</v>
       </c>
       <c r="V884" s="14" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="885" spans="4:22" x14ac:dyDescent="0.25">
@@ -29249,7 +29249,7 @@
         <v>0</v>
       </c>
       <c r="V888" s="14" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="889" spans="4:22" x14ac:dyDescent="0.25">
@@ -29284,7 +29284,7 @@
         <v>105</v>
       </c>
       <c r="V889" s="14" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="890" spans="4:22" x14ac:dyDescent="0.25">
@@ -29466,7 +29466,7 @@
         <v>0</v>
       </c>
       <c r="V896" s="14" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="897" spans="9:22" x14ac:dyDescent="0.25">
@@ -29519,7 +29519,7 @@
         <v>0</v>
       </c>
       <c r="V898" s="14" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="899" spans="9:22" x14ac:dyDescent="0.25">
@@ -29572,7 +29572,7 @@
         <v>0</v>
       </c>
       <c r="V900" s="14" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="901" spans="9:22" x14ac:dyDescent="0.25">
@@ -29625,7 +29625,7 @@
         <v>0</v>
       </c>
       <c r="V902" s="14" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="903" spans="9:22" x14ac:dyDescent="0.25">
@@ -30263,7 +30263,7 @@
         <v>0</v>
       </c>
       <c r="V928" s="14" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="929" spans="9:22" x14ac:dyDescent="0.25">
@@ -30340,7 +30340,7 @@
         <v>0</v>
       </c>
       <c r="V931" s="14" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="932" spans="9:22" x14ac:dyDescent="0.25">
@@ -30561,7 +30561,7 @@
         <v>0</v>
       </c>
       <c r="V940" s="14" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="941" spans="9:22" x14ac:dyDescent="0.25">
@@ -30590,7 +30590,7 @@
         <v>0</v>
       </c>
       <c r="V941" s="14" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="942" spans="9:22" x14ac:dyDescent="0.25">
@@ -30619,7 +30619,7 @@
         <v>0</v>
       </c>
       <c r="V942" s="14" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="943" spans="9:22" x14ac:dyDescent="0.25">
@@ -30648,7 +30648,7 @@
         <v>0</v>
       </c>
       <c r="V943" s="14" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="944" spans="9:22" x14ac:dyDescent="0.25">
@@ -30701,7 +30701,7 @@
         <v>0</v>
       </c>
       <c r="V945" s="14" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="946" spans="9:22" x14ac:dyDescent="0.25">
@@ -30758,7 +30758,7 @@
         <v>83</v>
       </c>
       <c r="V947" s="14" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="948" spans="9:22" x14ac:dyDescent="0.25">
@@ -31030,7 +31030,7 @@
         <v>96</v>
       </c>
       <c r="V958" s="14" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="959" spans="9:22" x14ac:dyDescent="0.25">
@@ -31107,7 +31107,7 @@
         <v>0</v>
       </c>
       <c r="V961" s="14" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="962" spans="9:22" x14ac:dyDescent="0.25">
@@ -31401,7 +31401,7 @@
         <v>84</v>
       </c>
       <c r="V973" s="14" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="974" spans="9:22" x14ac:dyDescent="0.25">
@@ -32265,7 +32265,7 @@
         <v>0</v>
       </c>
       <c r="V1008" s="14" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="1009" spans="4:22" x14ac:dyDescent="0.25">
@@ -32640,7 +32640,7 @@
         <v>83</v>
       </c>
       <c r="V1023" s="28" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="1024" spans="4:22" x14ac:dyDescent="0.25">
@@ -32820,7 +32820,7 @@
         <v>124</v>
       </c>
       <c r="D1030" s="48" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="H1030" s="47" t="s">
         <v>151</v>
@@ -32914,7 +32914,7 @@
     </row>
     <row r="1033" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D1033" s="48" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="H1033" s="47" t="s">
         <v>151</v>
@@ -33011,7 +33011,7 @@
         <v>83</v>
       </c>
       <c r="V1035" s="35" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="1036" spans="1:22" x14ac:dyDescent="0.25">
@@ -33089,7 +33089,7 @@
         <v>0</v>
       </c>
       <c r="V1038" s="14" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="1039" spans="1:22" x14ac:dyDescent="0.25">
@@ -33286,7 +33286,7 @@
         <v>0</v>
       </c>
       <c r="V1046" s="14" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="1047" spans="9:22" x14ac:dyDescent="0.25">
@@ -33315,7 +33315,7 @@
         <v>0</v>
       </c>
       <c r="V1047" s="14" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="1048" spans="9:22" x14ac:dyDescent="0.25">
@@ -33397,7 +33397,7 @@
         <v>0</v>
       </c>
       <c r="V1050" s="14" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="1051" spans="9:22" x14ac:dyDescent="0.25">
@@ -33499,7 +33499,7 @@
         <v>0</v>
       </c>
       <c r="V1054" s="14" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="1055" spans="9:22" x14ac:dyDescent="0.25">
@@ -33576,7 +33576,7 @@
         <v>83</v>
       </c>
       <c r="V1057" s="28" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="1058" spans="9:22" x14ac:dyDescent="0.25">
@@ -34362,7 +34362,7 @@
         <v>0</v>
       </c>
       <c r="V1088" s="14" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="1089" spans="9:22" x14ac:dyDescent="0.25">
@@ -34416,7 +34416,7 @@
         <v>0</v>
       </c>
       <c r="V1090" s="14" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="1091" spans="9:22" x14ac:dyDescent="0.25">
@@ -34445,7 +34445,7 @@
         <v>0</v>
       </c>
       <c r="V1091" s="14" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="1092" spans="9:22" x14ac:dyDescent="0.25">
@@ -34498,7 +34498,7 @@
         <v>0</v>
       </c>
       <c r="V1093" s="14" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="1094" spans="9:22" x14ac:dyDescent="0.25">
@@ -34575,7 +34575,7 @@
         <v>0</v>
       </c>
       <c r="V1096" s="14" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="1097" spans="9:22" x14ac:dyDescent="0.25">
@@ -34803,7 +34803,7 @@
     </row>
     <row r="1106" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F1106" s="54" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="G1106" s="47" t="s">
         <v>134</v>
@@ -34833,10 +34833,10 @@
     </row>
     <row r="1107" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B1107" s="54" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="F1107" s="54" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="G1107" s="47" t="s">
         <v>134</v>
@@ -35010,7 +35010,7 @@
         <v>83</v>
       </c>
       <c r="V1113" s="28" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="1114" spans="1:22" x14ac:dyDescent="0.25">
@@ -35217,7 +35217,7 @@
         <v>0</v>
       </c>
       <c r="V1121" s="14" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="1122" spans="8:22" x14ac:dyDescent="0.25">
@@ -35319,7 +35319,7 @@
         <v>0</v>
       </c>
       <c r="V1125" s="14" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="1126" spans="8:22" x14ac:dyDescent="0.25">
@@ -35398,7 +35398,7 @@
         <v>0</v>
       </c>
       <c r="V1128" s="14" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="1129" spans="8:22" x14ac:dyDescent="0.25">
@@ -35759,7 +35759,7 @@
         <v>83</v>
       </c>
       <c r="V1142" s="33" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="1143" spans="9:22" x14ac:dyDescent="0.25">
@@ -35836,7 +35836,7 @@
         <v>0</v>
       </c>
       <c r="V1145" s="14" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="1146" spans="9:22" x14ac:dyDescent="0.25">
@@ -35963,7 +35963,7 @@
         <v>83</v>
       </c>
       <c r="V1150" s="8" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="1151" spans="9:22" x14ac:dyDescent="0.25">
@@ -36064,12 +36064,12 @@
         <v>83</v>
       </c>
       <c r="V1154" s="35" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="1155" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1155" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="E1155" s="47" t="s">
         <v>132</v>
@@ -36100,7 +36100,7 @@
     </row>
     <row r="1156" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1156" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="E1156" s="47" t="s">
         <v>132</v>
@@ -36137,7 +36137,7 @@
     </row>
     <row r="1157" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1157" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="H1157" s="47" t="s">
         <v>154</v>
@@ -36167,7 +36167,7 @@
     </row>
     <row r="1158" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1158" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="H1158" s="47" t="s">
         <v>154</v>
@@ -36200,7 +36200,7 @@
     </row>
     <row r="1159" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1159" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1159" s="8" t="s">
         <v>41</v>
@@ -36228,7 +36228,7 @@
     </row>
     <row r="1160" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1160" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1160" s="8" t="s">
         <v>41</v>
@@ -36255,7 +36255,7 @@
     </row>
     <row r="1161" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1161" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1161" s="8" t="s">
         <v>41</v>
@@ -36283,7 +36283,7 @@
     </row>
     <row r="1162" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1162" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1162" s="8" t="s">
         <v>41</v>
@@ -36310,7 +36310,7 @@
     </row>
     <row r="1163" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1163" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1163" s="8" t="s">
         <v>41</v>
@@ -36337,7 +36337,7 @@
     </row>
     <row r="1164" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1164" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1164" s="8" t="s">
         <v>41</v>
@@ -36364,7 +36364,7 @@
     </row>
     <row r="1165" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1165" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1165" s="8" t="s">
         <v>41</v>
@@ -36391,12 +36391,12 @@
         <v>83</v>
       </c>
       <c r="V1165" s="8" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="1166" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1166" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1166" s="8" t="s">
         <v>41</v>
@@ -36423,7 +36423,7 @@
     </row>
     <row r="1167" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1167" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1167" s="8" t="s">
         <v>41</v>
@@ -36450,7 +36450,7 @@
     </row>
     <row r="1168" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1168" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1168" s="8" t="s">
         <v>41</v>
@@ -36478,7 +36478,7 @@
     </row>
     <row r="1169" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1169" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1169" s="8" t="s">
         <v>41</v>
@@ -36505,7 +36505,7 @@
     </row>
     <row r="1170" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1170" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1170" s="8" t="s">
         <v>41</v>
@@ -36532,12 +36532,12 @@
         <v>0</v>
       </c>
       <c r="V1170" s="14" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="1171" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1171" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1171" s="8" t="s">
         <v>41</v>
@@ -36564,7 +36564,7 @@
     </row>
     <row r="1172" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1172" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1172" s="8" t="s">
         <v>41</v>
@@ -36591,7 +36591,7 @@
     </row>
     <row r="1173" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1173" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1173" s="8" t="s">
         <v>41</v>
@@ -36618,12 +36618,12 @@
         <v>0</v>
       </c>
       <c r="V1173" s="14" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="1174" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1174" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1174" s="8" t="s">
         <v>41</v>
@@ -36650,7 +36650,7 @@
     </row>
     <row r="1175" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1175" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1175" s="8" t="s">
         <v>41</v>
@@ -36677,7 +36677,7 @@
     </row>
     <row r="1176" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1176" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1176" s="8" t="s">
         <v>41</v>
@@ -36709,7 +36709,7 @@
     </row>
     <row r="1177" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1177" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1177" s="8" t="s">
         <v>41</v>
@@ -36739,7 +36739,7 @@
     </row>
     <row r="1178" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1178" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1178" s="8" t="s">
         <v>41</v>
@@ -36766,7 +36766,7 @@
     </row>
     <row r="1179" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1179" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1179" s="8" t="s">
         <v>41</v>
@@ -36793,7 +36793,7 @@
     </row>
     <row r="1180" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1180" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1180" s="8" t="s">
         <v>41</v>
@@ -36820,7 +36820,7 @@
     </row>
     <row r="1181" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1181" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1181" s="8" t="s">
         <v>41</v>
@@ -36847,7 +36847,7 @@
     </row>
     <row r="1182" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1182" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1182" s="8" t="s">
         <v>41</v>
@@ -36874,7 +36874,7 @@
     </row>
     <row r="1183" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1183" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1183" s="8" t="s">
         <v>41</v>
@@ -36901,12 +36901,12 @@
         <v>0</v>
       </c>
       <c r="V1183" s="14" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="1184" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1184" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1184" s="8" t="s">
         <v>41</v>
@@ -36933,12 +36933,12 @@
         <v>83</v>
       </c>
       <c r="V1184" s="35" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="1185" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1185" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1185" s="8" t="s">
         <v>41</v>
@@ -36965,7 +36965,7 @@
     </row>
     <row r="1186" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1186" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1186" s="8" t="s">
         <v>41</v>
@@ -36992,7 +36992,7 @@
     </row>
     <row r="1187" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1187" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1187" s="8" t="s">
         <v>41</v>
@@ -37019,7 +37019,7 @@
     </row>
     <row r="1188" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1188" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1188" s="8" t="s">
         <v>41</v>
@@ -37046,7 +37046,7 @@
     </row>
     <row r="1189" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1189" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1189" s="8" t="s">
         <v>41</v>
@@ -37073,12 +37073,12 @@
         <v>0</v>
       </c>
       <c r="V1189" s="14" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="1190" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1190" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1190" s="8" t="s">
         <v>41</v>
@@ -37105,7 +37105,7 @@
     </row>
     <row r="1191" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1191" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1191" s="8" t="s">
         <v>41</v>
@@ -37132,12 +37132,12 @@
         <v>83</v>
       </c>
       <c r="V1191" s="28" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="1192" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1192" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1192" s="8" t="s">
         <v>41</v>
@@ -37164,7 +37164,7 @@
     </row>
     <row r="1193" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1193" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1193" s="8" t="s">
         <v>41</v>
@@ -37191,7 +37191,7 @@
     </row>
     <row r="1194" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1194" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1194" s="8" t="s">
         <v>41</v>
@@ -37221,10 +37221,10 @@
     </row>
     <row r="1195" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1195" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="F1195" s="54" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="I1195" s="8" t="s">
         <v>41</v>
@@ -37248,7 +37248,7 @@
         <v>831</v>
       </c>
       <c r="S1195" s="41" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="T1195" s="2" t="s">
         <v>114</v>
@@ -37260,10 +37260,10 @@
         <v>124</v>
       </c>
       <c r="C1196" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="F1196" s="54" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="I1196" s="8" t="s">
         <v>41</v>
@@ -37290,7 +37290,7 @@
     </row>
     <row r="1197" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1197" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1197" s="8" t="s">
         <v>41</v>
@@ -37317,12 +37317,12 @@
         <v>0</v>
       </c>
       <c r="V1197" s="14" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="1198" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1198" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1198" s="8" t="s">
         <v>41</v>
@@ -37349,7 +37349,7 @@
     </row>
     <row r="1199" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1199" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1199" s="8" t="s">
         <v>41</v>
@@ -37376,7 +37376,7 @@
     </row>
     <row r="1200" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1200" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1200" s="8" t="s">
         <v>41</v>
@@ -37403,7 +37403,7 @@
     </row>
     <row r="1201" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1201" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1201" s="8" t="s">
         <v>41</v>
@@ -37430,12 +37430,12 @@
         <v>83</v>
       </c>
       <c r="V1201" s="28" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="1202" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1202" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1202" s="8" t="s">
         <v>41</v>
@@ -37463,7 +37463,7 @@
     </row>
     <row r="1203" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1203" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1203" s="8" t="s">
         <v>41</v>
@@ -37490,7 +37490,7 @@
     </row>
     <row r="1204" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1204" s="49" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="H1204" s="47" t="s">
         <v>155</v>
@@ -37520,7 +37520,7 @@
         <v>0</v>
       </c>
       <c r="V1204" s="14" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="1205" spans="3:22" x14ac:dyDescent="0.25">
@@ -37551,7 +37551,7 @@
         <v>0</v>
       </c>
       <c r="V1205" s="32" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="1206" spans="3:22" x14ac:dyDescent="0.25">
@@ -37686,7 +37686,7 @@
         <v>83</v>
       </c>
       <c r="V1210" s="8" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="1211" spans="3:22" x14ac:dyDescent="0.25">
@@ -37772,7 +37772,7 @@
         <v>0</v>
       </c>
       <c r="V1213" s="14" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="1214" spans="3:22" x14ac:dyDescent="0.25">
@@ -37926,7 +37926,7 @@
         <v>83</v>
       </c>
       <c r="V1219" s="8" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="1220" spans="4:22" x14ac:dyDescent="0.25">
@@ -38175,7 +38175,7 @@
         <v>0</v>
       </c>
       <c r="V1228" s="14" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="1229" spans="4:22" x14ac:dyDescent="0.25">
@@ -38459,7 +38459,7 @@
         <v>83</v>
       </c>
       <c r="V1239" s="14" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="1240" spans="8:22" x14ac:dyDescent="0.25">
@@ -38712,7 +38712,7 @@
         <v>15</v>
       </c>
       <c r="V1248" s="26" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="1249" spans="9:22" x14ac:dyDescent="0.25">
@@ -38824,7 +38824,7 @@
         <v>15</v>
       </c>
       <c r="V1252" s="28" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="1253" spans="9:22" x14ac:dyDescent="0.25">
@@ -38877,7 +38877,7 @@
         <v>0</v>
       </c>
       <c r="V1254" s="14" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="1255" spans="9:22" x14ac:dyDescent="0.25">
@@ -39034,7 +39034,7 @@
         <v>83</v>
       </c>
       <c r="V1260" s="31" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="1261" spans="9:22" x14ac:dyDescent="0.25">
@@ -39258,7 +39258,7 @@
         <v>83</v>
       </c>
       <c r="V1269" s="28" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="1270" spans="9:22" x14ac:dyDescent="0.25">
@@ -39337,7 +39337,7 @@
         <v>0</v>
       </c>
       <c r="V1272" s="14" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="1273" spans="9:22" x14ac:dyDescent="0.25">
@@ -39390,7 +39390,7 @@
         <v>0</v>
       </c>
       <c r="V1274" s="14" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="1275" spans="9:22" x14ac:dyDescent="0.25">
@@ -39419,7 +39419,7 @@
         <v>83</v>
       </c>
       <c r="V1275" s="35" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="1276" spans="9:22" x14ac:dyDescent="0.25">
@@ -39497,7 +39497,7 @@
         <v>83</v>
       </c>
       <c r="V1278" s="28" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="1279" spans="9:22" x14ac:dyDescent="0.25">
@@ -39745,7 +39745,7 @@
         <v>0</v>
       </c>
       <c r="V1287" s="14" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="1288" spans="1:22" x14ac:dyDescent="0.25">
@@ -39780,7 +39780,7 @@
         <v>83</v>
       </c>
       <c r="V1288" s="14" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="1289" spans="1:22" x14ac:dyDescent="0.25">
@@ -40020,7 +40020,7 @@
         <v>83</v>
       </c>
       <c r="V1297" s="28" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="1298" spans="8:22" x14ac:dyDescent="0.25">
@@ -40145,7 +40145,7 @@
         <v>0</v>
       </c>
       <c r="V1302" s="14" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="1303" spans="8:22" x14ac:dyDescent="0.25">
@@ -40201,7 +40201,7 @@
         <v>83</v>
       </c>
       <c r="V1304" s="35" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="1305" spans="8:22" x14ac:dyDescent="0.25">
@@ -40229,7 +40229,7 @@
         <v>15</v>
       </c>
       <c r="V1305" s="26" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="1306" spans="8:22" x14ac:dyDescent="0.25">
@@ -40258,7 +40258,7 @@
         <v>0</v>
       </c>
       <c r="V1306" s="14" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="1307" spans="8:22" x14ac:dyDescent="0.25">
@@ -40287,7 +40287,7 @@
         <v>83</v>
       </c>
       <c r="V1307" s="35" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="1308" spans="8:22" x14ac:dyDescent="0.25">
@@ -40388,7 +40388,7 @@
         <v>0</v>
       </c>
       <c r="V1311" s="14" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="1312" spans="8:22" x14ac:dyDescent="0.25">
@@ -40441,7 +40441,7 @@
         <v>0</v>
       </c>
       <c r="V1313" s="14" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1314" spans="9:22" x14ac:dyDescent="0.25">
@@ -40547,7 +40547,7 @@
         <v>0</v>
       </c>
       <c r="V1317" s="14" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="1318" spans="9:22" x14ac:dyDescent="0.25">
@@ -40648,7 +40648,7 @@
         <v>0</v>
       </c>
       <c r="V1321" s="14" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="1322" spans="9:22" x14ac:dyDescent="0.25">
@@ -40677,7 +40677,7 @@
         <v>83</v>
       </c>
       <c r="V1322" s="31" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="1323" spans="9:22" x14ac:dyDescent="0.25">
@@ -40706,7 +40706,7 @@
         <v>90</v>
       </c>
       <c r="T1323" s="2" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="V1323" s="14"/>
     </row>
@@ -40860,7 +40860,7 @@
         <v>83</v>
       </c>
       <c r="V1329" s="28" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="1330" spans="4:22" x14ac:dyDescent="0.25">
@@ -41015,7 +41015,7 @@
         <v>181</v>
       </c>
       <c r="N1335" s="55" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="O1335" s="1" t="s">
         <v>103</v>
@@ -41098,7 +41098,7 @@
         <v>83</v>
       </c>
       <c r="V1338" s="26" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="1339" spans="4:22" x14ac:dyDescent="0.25">
@@ -41136,7 +41136,7 @@
         <v>0</v>
       </c>
       <c r="V1339" s="14" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="1340" spans="4:22" x14ac:dyDescent="0.25">
@@ -41249,7 +41249,7 @@
         <v>0</v>
       </c>
       <c r="V1343" s="14" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="1344" spans="4:22" x14ac:dyDescent="0.25">
@@ -41278,7 +41278,7 @@
         <v>0</v>
       </c>
       <c r="V1344" s="14" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="1345" spans="9:22" x14ac:dyDescent="0.25">
@@ -41307,7 +41307,7 @@
         <v>83</v>
       </c>
       <c r="V1345" s="28" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="1346" spans="9:22" x14ac:dyDescent="0.25">
@@ -41580,7 +41580,7 @@
         <v>83</v>
       </c>
       <c r="V1356" s="35" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="1357" spans="9:22" x14ac:dyDescent="0.25">
@@ -41658,7 +41658,7 @@
         <v>0</v>
       </c>
       <c r="V1359" s="14" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="1360" spans="9:22" x14ac:dyDescent="0.25">
@@ -41687,7 +41687,7 @@
         <v>0</v>
       </c>
       <c r="V1360" s="14" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="1361" spans="4:22" x14ac:dyDescent="0.25">
@@ -41719,7 +41719,7 @@
         <v>83</v>
       </c>
       <c r="V1361" s="14" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="1362" spans="4:22" x14ac:dyDescent="0.25">
@@ -41800,7 +41800,7 @@
         <v>83</v>
       </c>
       <c r="V1364" s="14" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="1365" spans="4:22" x14ac:dyDescent="0.25">
@@ -42045,7 +42045,7 @@
         <v>83</v>
       </c>
       <c r="V1373" s="14" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="1374" spans="4:22" x14ac:dyDescent="0.25">
@@ -42098,7 +42098,7 @@
         <v>0</v>
       </c>
       <c r="V1375" s="14" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="1376" spans="4:22" x14ac:dyDescent="0.25">
@@ -42133,7 +42133,7 @@
       <c r="T1376" s="43"/>
       <c r="U1376" s="43"/>
       <c r="V1376" s="14" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1377" spans="8:22" x14ac:dyDescent="0.25">
@@ -42271,7 +42271,7 @@
         <v>83</v>
       </c>
       <c r="V1381" s="14" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="1382" spans="8:22" x14ac:dyDescent="0.25">
@@ -42447,7 +42447,7 @@
         <v>83</v>
       </c>
       <c r="V1388" s="28" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="1389" spans="8:22" x14ac:dyDescent="0.25">
@@ -42527,7 +42527,7 @@
         <v>83</v>
       </c>
       <c r="V1391" s="14" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="1392" spans="8:22" x14ac:dyDescent="0.25">
@@ -42681,7 +42681,7 @@
         <v>0</v>
       </c>
       <c r="V1397" s="14" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="1398" spans="9:22" x14ac:dyDescent="0.25">
@@ -42758,7 +42758,7 @@
         <v>83</v>
       </c>
       <c r="V1400" s="28" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="1401" spans="9:22" x14ac:dyDescent="0.25">
@@ -42868,7 +42868,7 @@
         <v>0</v>
       </c>
       <c r="V1404" s="14" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="1405" spans="9:22" x14ac:dyDescent="0.25">
@@ -42995,7 +42995,7 @@
         <v>83</v>
       </c>
       <c r="V1409" s="14" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="1410" spans="9:22" x14ac:dyDescent="0.25">
@@ -43099,7 +43099,7 @@
         <v>0</v>
       </c>
       <c r="V1413" s="14" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="1414" spans="9:22" x14ac:dyDescent="0.25">
@@ -43223,7 +43223,7 @@
         <v>0</v>
       </c>
       <c r="V1418" s="8" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="1419" spans="9:22" x14ac:dyDescent="0.25">
@@ -43280,7 +43280,7 @@
         <v>96</v>
       </c>
       <c r="V1420" s="35" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="1421" spans="9:22" x14ac:dyDescent="0.25">
@@ -43406,7 +43406,7 @@
         <v>0</v>
       </c>
       <c r="V1425" s="14" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="1426" spans="8:22" x14ac:dyDescent="0.25">
@@ -43657,7 +43657,7 @@
         <v>0</v>
       </c>
       <c r="V1435" s="14" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="1436" spans="8:22" x14ac:dyDescent="0.25">
@@ -43689,7 +43689,7 @@
         <v>83</v>
       </c>
       <c r="V1436" s="28" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="1437" spans="8:22" x14ac:dyDescent="0.25">
@@ -43775,7 +43775,7 @@
         <v>0</v>
       </c>
       <c r="V1439" s="14" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="1440" spans="8:22" x14ac:dyDescent="0.25">
@@ -43804,7 +43804,7 @@
         <v>0</v>
       </c>
       <c r="V1440" s="14" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="1441" spans="1:22" x14ac:dyDescent="0.25">
@@ -43881,7 +43881,7 @@
         <v>0</v>
       </c>
       <c r="V1443" s="14" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="1444" spans="1:22" x14ac:dyDescent="0.25">
@@ -43934,7 +43934,7 @@
         <v>83</v>
       </c>
       <c r="V1445" s="32" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="1446" spans="1:22" x14ac:dyDescent="0.25">
@@ -44086,7 +44086,7 @@
         <v>0</v>
       </c>
       <c r="V1451" s="14" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="1452" spans="1:22" x14ac:dyDescent="0.25">
@@ -44115,7 +44115,7 @@
         <v>83</v>
       </c>
       <c r="V1452" s="28" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="1453" spans="1:22" x14ac:dyDescent="0.25">
@@ -44195,7 +44195,7 @@
     </row>
     <row r="1456" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1456" s="51" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="H1456" s="47" t="s">
         <v>161</v>
@@ -44228,7 +44228,7 @@
     </row>
     <row r="1457" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1457" s="51" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="H1457" s="47" t="s">
         <v>161</v>
@@ -44312,7 +44312,7 @@
         <v>83</v>
       </c>
       <c r="V1459" s="28" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="1460" spans="1:22" x14ac:dyDescent="0.25">
@@ -44392,7 +44392,7 @@
         <v>0</v>
       </c>
       <c r="V1462" s="14" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="1463" spans="1:22" x14ac:dyDescent="0.25">
@@ -44496,7 +44496,7 @@
         <v>83</v>
       </c>
       <c r="V1466" s="35" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="1467" spans="1:22" x14ac:dyDescent="0.25">
@@ -44675,7 +44675,7 @@
         <v>83</v>
       </c>
       <c r="V1473" s="14" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="1474" spans="6:22" x14ac:dyDescent="0.25">
@@ -44704,7 +44704,7 @@
         <v>0</v>
       </c>
       <c r="V1474" s="14" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="1475" spans="6:22" x14ac:dyDescent="0.25">
@@ -44733,7 +44733,7 @@
         <v>0</v>
       </c>
       <c r="V1475" s="14" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1476" spans="6:22" x14ac:dyDescent="0.25">
@@ -44762,7 +44762,7 @@
         <v>0</v>
       </c>
       <c r="V1476" s="14" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="1477" spans="6:22" x14ac:dyDescent="0.25">
@@ -44791,7 +44791,7 @@
         <v>83</v>
       </c>
       <c r="V1477" s="8" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="1478" spans="6:22" x14ac:dyDescent="0.25">
@@ -44871,12 +44871,12 @@
         <v>96</v>
       </c>
       <c r="V1480" s="28" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="1481" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F1481" s="54" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="H1481" s="47" t="s">
         <v>162</v>
@@ -44906,7 +44906,7 @@
     </row>
     <row r="1482" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F1482" s="54" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="H1482" s="47" t="s">
         <v>162</v>
@@ -44963,7 +44963,7 @@
         <v>15</v>
       </c>
       <c r="V1483" s="26" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="1484" spans="6:22" x14ac:dyDescent="0.25">
@@ -45025,7 +45025,7 @@
         <v>0</v>
       </c>
       <c r="V1485" s="14" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="1486" spans="6:22" x14ac:dyDescent="0.25">
@@ -45158,7 +45158,7 @@
         <v>83</v>
       </c>
       <c r="V1490" s="28" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="1491" spans="8:22" x14ac:dyDescent="0.25">
@@ -45259,7 +45259,7 @@
         <v>0</v>
       </c>
       <c r="V1494" s="14" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="1495" spans="8:22" x14ac:dyDescent="0.25">
@@ -45480,7 +45480,7 @@
         <v>123</v>
       </c>
       <c r="V1502" s="28" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="1503" spans="8:22" x14ac:dyDescent="0.25">
@@ -45781,7 +45781,7 @@
         <v>83</v>
       </c>
       <c r="V1514" s="28" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="1515" spans="5:22" x14ac:dyDescent="0.25">
@@ -45810,7 +45810,7 @@
     </row>
     <row r="1516" spans="5:22" x14ac:dyDescent="0.25">
       <c r="F1516" s="54" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="I1516" s="8" t="s">
         <v>48</v>
@@ -45837,7 +45837,7 @@
     </row>
     <row r="1517" spans="5:22" x14ac:dyDescent="0.25">
       <c r="F1517" s="54" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="I1517" s="8" t="s">
         <v>48</v>
@@ -45864,7 +45864,7 @@
         <v>0</v>
       </c>
       <c r="V1517" s="14" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="1518" spans="5:22" x14ac:dyDescent="0.25">
@@ -45872,7 +45872,7 @@
         <v>132</v>
       </c>
       <c r="F1518" s="54" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="I1518" s="8" t="s">
         <v>48</v>
@@ -45902,7 +45902,7 @@
         <v>100</v>
       </c>
       <c r="V1518" s="26" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="1519" spans="5:22" x14ac:dyDescent="0.25">
@@ -45910,7 +45910,7 @@
         <v>132</v>
       </c>
       <c r="F1519" s="54" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="I1519" s="8" t="s">
         <v>48</v>
@@ -45964,7 +45964,7 @@
         <v>83</v>
       </c>
       <c r="V1520" s="14" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="1521" spans="1:22" x14ac:dyDescent="0.25">
@@ -46347,7 +46347,7 @@
         <v>83</v>
       </c>
       <c r="V1535" s="36" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="1536" spans="1:22" x14ac:dyDescent="0.25">
@@ -46577,7 +46577,7 @@
         <v>83</v>
       </c>
       <c r="V1544" s="28" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="1545" spans="8:22" x14ac:dyDescent="0.25">
@@ -46764,7 +46764,7 @@
         <v>0</v>
       </c>
       <c r="V1551" s="14" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="1552" spans="8:22" x14ac:dyDescent="0.25">
@@ -46865,7 +46865,7 @@
         <v>83</v>
       </c>
       <c r="V1555" s="8" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="1556" spans="5:22" x14ac:dyDescent="0.25">
@@ -46945,7 +46945,7 @@
         <v>83</v>
       </c>
       <c r="V1558" s="14" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="1559" spans="5:22" x14ac:dyDescent="0.25">
@@ -47125,7 +47125,7 @@
         <v>83</v>
       </c>
       <c r="V1565" s="28" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="1566" spans="5:22" x14ac:dyDescent="0.25">
@@ -47206,7 +47206,7 @@
         <v>96</v>
       </c>
       <c r="V1568" s="32" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nmv 27 02 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.3 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34860340-728C-4387-BFC5-ACEA56C30570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377A95BD-BF4C-47B7-AC4B-8F61BFE1D3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4275" uniqueCount="1330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4274" uniqueCount="1330">
   <si>
     <t>PS</t>
   </si>
@@ -4751,10 +4751,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1568"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A271" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A478" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="V279" sqref="V279"/>
+      <selection pane="bottomLeft" activeCell="U483" sqref="U483"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -18807,9 +18807,6 @@
       <c r="N483" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="U483" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="V483" s="14"/>
     </row>
     <row r="484" spans="9:22" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
nmv 28 07 2025
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.3 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA519FD4-D0B8-4D7B-AF40-8A377A9E8EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECA6263-0480-43DE-B601-3AC64BAAEC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3484,9 +3484,6 @@
   </si>
   <si>
     <t xml:space="preserve">samo#kasAqvitiq saM - oqkaqsauq </t>
-  </si>
-  <si>
-    <t xml:space="preserve">aqreqpasAvitya#reqpasau$ </t>
   </si>
   <si>
     <t xml:space="preserve">jAqtaqveqdaqsAqviti# jAta - veqdaqsauq </t>
@@ -4078,6 +4075,9 @@
   </si>
   <si>
     <t xml:space="preserve">iqndriqyAvAn# </t>
+  </si>
+  <si>
+    <t xml:space="preserve">aqreqpasAqvitya#reqpasau$ </t>
   </si>
 </sst>
 </file>
@@ -4751,10 +4751,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1568"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1111" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A637" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="N1115" sqref="N1115"/>
+      <selection pane="bottomLeft" activeCell="X641" sqref="X641"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -5226,7 +5226,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="72" x14ac:dyDescent="0.25">
       <c r="A1" s="50" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15" t="s">
@@ -5278,10 +5278,10 @@
         <v>10</v>
       </c>
       <c r="S1" s="39" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="T1" s="39" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="U1" s="38" t="s">
         <v>17</v>
@@ -5432,7 +5432,7 @@
         <v>4</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>0</v>
@@ -13112,7 +13112,7 @@
     </row>
     <row r="264" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A264" s="51" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="H264" s="47" t="s">
         <v>137</v>
@@ -13142,7 +13142,7 @@
     </row>
     <row r="265" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A265" s="51" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="H265" s="47" t="s">
         <v>137</v>
@@ -13532,7 +13532,7 @@
         <v>82</v>
       </c>
       <c r="V279" s="57" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="280" spans="1:22" x14ac:dyDescent="0.25">
@@ -13641,7 +13641,7 @@
     </row>
     <row r="284" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A284" s="51" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="H284" s="47" t="s">
         <v>138</v>
@@ -13676,7 +13676,7 @@
     </row>
     <row r="285" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A285" s="51" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="H285" s="47" t="s">
         <v>138</v>
@@ -13931,7 +13931,7 @@
     </row>
     <row r="295" spans="4:22" x14ac:dyDescent="0.25">
       <c r="F295" s="54" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="I295" s="8" t="s">
         <v>23</v>
@@ -13958,7 +13958,7 @@
     </row>
     <row r="296" spans="4:22" x14ac:dyDescent="0.25">
       <c r="F296" s="54" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="I296" s="8" t="s">
         <v>23</v>
@@ -13989,7 +13989,7 @@
         <v>127</v>
       </c>
       <c r="F297" s="54" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="I297" s="8" t="s">
         <v>23</v>
@@ -14019,7 +14019,7 @@
     </row>
     <row r="298" spans="4:22" x14ac:dyDescent="0.25">
       <c r="F298" s="54" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="I298" s="8" t="s">
         <v>23</v>
@@ -15841,7 +15841,7 @@
     </row>
     <row r="368" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D368" s="48" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="H368" s="47" t="s">
         <v>140</v>
@@ -20375,7 +20375,7 @@
         <v>82</v>
       </c>
       <c r="V544" s="59" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="545" spans="9:22" x14ac:dyDescent="0.25">
@@ -22429,7 +22429,7 @@
         <v>95</v>
       </c>
       <c r="V625" s="59" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="626" spans="1:22" x14ac:dyDescent="0.25">
@@ -22911,8 +22911,8 @@
       <c r="P643" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="V643" s="32" t="s">
-        <v>1152</v>
+      <c r="V643" s="57" t="s">
+        <v>1329</v>
       </c>
     </row>
     <row r="644" spans="5:22" x14ac:dyDescent="0.25">
@@ -23067,7 +23067,7 @@
         <v>0</v>
       </c>
       <c r="V649" s="14" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="650" spans="5:22" x14ac:dyDescent="0.25">
@@ -23121,10 +23121,10 @@
     </row>
     <row r="652" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E652" s="54" t="s">
+        <v>1309</v>
+      </c>
+      <c r="F652" s="54" t="s">
         <v>1310</v>
-      </c>
-      <c r="F652" s="54" t="s">
-        <v>1311</v>
       </c>
       <c r="I652" s="8" t="s">
         <v>30</v>
@@ -23151,10 +23151,10 @@
     </row>
     <row r="653" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E653" s="54" t="s">
+        <v>1309</v>
+      </c>
+      <c r="F653" s="54" t="s">
         <v>1310</v>
-      </c>
-      <c r="F653" s="54" t="s">
-        <v>1311</v>
       </c>
       <c r="I653" s="8" t="s">
         <v>30</v>
@@ -23181,7 +23181,7 @@
         <v>82</v>
       </c>
       <c r="V653" s="24" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="654" spans="5:22" x14ac:dyDescent="0.25">
@@ -23283,7 +23283,7 @@
         <v>0</v>
       </c>
       <c r="V657" s="14" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="658" spans="8:22" x14ac:dyDescent="0.25">
@@ -23363,7 +23363,7 @@
         <v>88</v>
       </c>
       <c r="V660" s="14" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="661" spans="8:22" x14ac:dyDescent="0.25">
@@ -23392,7 +23392,7 @@
         <v>82</v>
       </c>
       <c r="V661" s="57" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="662" spans="8:22" x14ac:dyDescent="0.25">
@@ -23421,7 +23421,7 @@
         <v>0</v>
       </c>
       <c r="V662" s="14" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="663" spans="8:22" x14ac:dyDescent="0.25">
@@ -23643,7 +23643,7 @@
         <v>82</v>
       </c>
       <c r="V670" s="14" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="671" spans="8:22" x14ac:dyDescent="0.25">
@@ -23769,7 +23769,7 @@
         <v>0</v>
       </c>
       <c r="V675" s="14" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="676" spans="9:22" x14ac:dyDescent="0.25">
@@ -23925,7 +23925,7 @@
         <v>0</v>
       </c>
       <c r="V681" s="14" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="682" spans="9:22" x14ac:dyDescent="0.25">
@@ -24178,7 +24178,7 @@
         <v>0</v>
       </c>
       <c r="V691" s="14" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="692" spans="9:22" x14ac:dyDescent="0.25">
@@ -24379,7 +24379,7 @@
         <v>0</v>
       </c>
       <c r="V699" s="14" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="700" spans="9:22" x14ac:dyDescent="0.25">
@@ -24558,7 +24558,7 @@
         <v>0</v>
       </c>
       <c r="V706" s="14" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="707" spans="5:22" x14ac:dyDescent="0.25">
@@ -24587,7 +24587,7 @@
         <v>0</v>
       </c>
       <c r="V707" s="14" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="708" spans="5:22" x14ac:dyDescent="0.25">
@@ -24714,7 +24714,7 @@
     </row>
     <row r="713" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E713" s="54" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="H713" s="47" t="s">
         <v>146</v>
@@ -24752,7 +24752,7 @@
     </row>
     <row r="714" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E714" s="54" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="H714" s="47" t="s">
         <v>146</v>
@@ -24785,12 +24785,12 @@
         <v>92</v>
       </c>
       <c r="V714" s="14" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="715" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E715" s="54" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="H715" s="47" t="s">
         <v>146</v>
@@ -24823,7 +24823,7 @@
     </row>
     <row r="716" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E716" s="54" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="H716" s="47" t="s">
         <v>146</v>
@@ -24933,7 +24933,7 @@
         <v>0</v>
       </c>
       <c r="V719" s="14" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="720" spans="5:22" x14ac:dyDescent="0.25">
@@ -25354,7 +25354,7 @@
         <v>0</v>
       </c>
       <c r="V736" s="14" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="737" spans="8:22" x14ac:dyDescent="0.25">
@@ -25464,7 +25464,7 @@
         <v>0</v>
       </c>
       <c r="V740" s="14" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="741" spans="8:22" x14ac:dyDescent="0.25">
@@ -25837,7 +25837,7 @@
         <v>0</v>
       </c>
       <c r="V754" s="32" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="755" spans="9:22" x14ac:dyDescent="0.25">
@@ -26016,7 +26016,7 @@
         <v>0</v>
       </c>
       <c r="V761" s="14" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="762" spans="9:22" x14ac:dyDescent="0.25">
@@ -26045,7 +26045,7 @@
         <v>0</v>
       </c>
       <c r="V762" s="14" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="763" spans="9:22" x14ac:dyDescent="0.25">
@@ -26098,7 +26098,7 @@
         <v>82</v>
       </c>
       <c r="V764" s="35" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="765" spans="9:22" x14ac:dyDescent="0.25">
@@ -26225,7 +26225,7 @@
         <v>0</v>
       </c>
       <c r="V769" s="14" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="770" spans="8:22" x14ac:dyDescent="0.25">
@@ -26592,7 +26592,7 @@
         <v>119</v>
       </c>
       <c r="V783" s="14" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="784" spans="8:22" x14ac:dyDescent="0.25">
@@ -26871,7 +26871,7 @@
         <v>0</v>
       </c>
       <c r="V794" s="14" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="795" spans="4:22" x14ac:dyDescent="0.25">
@@ -27368,7 +27368,7 @@
         <v>0</v>
       </c>
       <c r="V814" s="14" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="815" spans="9:22" x14ac:dyDescent="0.25">
@@ -27523,7 +27523,7 @@
         <v>0</v>
       </c>
       <c r="V820" s="14" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="821" spans="9:22" x14ac:dyDescent="0.25">
@@ -28705,7 +28705,7 @@
         <v>0</v>
       </c>
       <c r="V867" s="14" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="868" spans="8:22" x14ac:dyDescent="0.25">
@@ -28758,7 +28758,7 @@
         <v>82</v>
       </c>
       <c r="V869" s="35" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="870" spans="8:22" x14ac:dyDescent="0.25">
@@ -28912,7 +28912,7 @@
         <v>0</v>
       </c>
       <c r="V875" s="14" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="876" spans="8:22" x14ac:dyDescent="0.25">
@@ -28941,7 +28941,7 @@
         <v>0</v>
       </c>
       <c r="V876" s="14" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="877" spans="8:22" x14ac:dyDescent="0.25">
@@ -29036,13 +29036,13 @@
         <v>11</v>
       </c>
       <c r="N880" s="5" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="O880" s="2" t="s">
         <v>0</v>
       </c>
       <c r="V880" s="14" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="881" spans="4:22" x14ac:dyDescent="0.25">
@@ -29119,7 +29119,7 @@
         <v>0</v>
       </c>
       <c r="V883" s="14" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="884" spans="4:22" x14ac:dyDescent="0.25">
@@ -29154,7 +29154,7 @@
         <v>104</v>
       </c>
       <c r="V884" s="14" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="885" spans="4:22" x14ac:dyDescent="0.25">
@@ -29258,7 +29258,7 @@
         <v>0</v>
       </c>
       <c r="V888" s="14" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="889" spans="4:22" x14ac:dyDescent="0.25">
@@ -29293,7 +29293,7 @@
         <v>104</v>
       </c>
       <c r="V889" s="14" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="890" spans="4:22" x14ac:dyDescent="0.25">
@@ -29475,7 +29475,7 @@
         <v>0</v>
       </c>
       <c r="V896" s="14" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="897" spans="9:22" x14ac:dyDescent="0.25">
@@ -29528,7 +29528,7 @@
         <v>0</v>
       </c>
       <c r="V898" s="14" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="899" spans="9:22" x14ac:dyDescent="0.25">
@@ -29581,7 +29581,7 @@
         <v>0</v>
       </c>
       <c r="V900" s="14" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="901" spans="9:22" x14ac:dyDescent="0.25">
@@ -29634,7 +29634,7 @@
         <v>0</v>
       </c>
       <c r="V902" s="14" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="903" spans="9:22" x14ac:dyDescent="0.25">
@@ -30272,7 +30272,7 @@
         <v>0</v>
       </c>
       <c r="V928" s="14" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="929" spans="9:22" x14ac:dyDescent="0.25">
@@ -30349,7 +30349,7 @@
         <v>0</v>
       </c>
       <c r="V931" s="14" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="932" spans="9:22" x14ac:dyDescent="0.25">
@@ -30570,7 +30570,7 @@
         <v>0</v>
       </c>
       <c r="V940" s="14" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="941" spans="9:22" x14ac:dyDescent="0.25">
@@ -30599,7 +30599,7 @@
         <v>0</v>
       </c>
       <c r="V941" s="14" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="942" spans="9:22" x14ac:dyDescent="0.25">
@@ -30628,7 +30628,7 @@
         <v>0</v>
       </c>
       <c r="V942" s="14" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="943" spans="9:22" x14ac:dyDescent="0.25">
@@ -30657,7 +30657,7 @@
         <v>0</v>
       </c>
       <c r="V943" s="14" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="944" spans="9:22" x14ac:dyDescent="0.25">
@@ -30710,7 +30710,7 @@
         <v>0</v>
       </c>
       <c r="V945" s="14" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="946" spans="9:22" x14ac:dyDescent="0.25">
@@ -30767,7 +30767,7 @@
         <v>82</v>
       </c>
       <c r="V947" s="14" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="948" spans="9:22" x14ac:dyDescent="0.25">
@@ -31039,7 +31039,7 @@
         <v>95</v>
       </c>
       <c r="V958" s="14" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="959" spans="9:22" x14ac:dyDescent="0.25">
@@ -31116,7 +31116,7 @@
         <v>0</v>
       </c>
       <c r="V961" s="14" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="962" spans="9:22" x14ac:dyDescent="0.25">
@@ -31410,7 +31410,7 @@
         <v>83</v>
       </c>
       <c r="V973" s="14" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="974" spans="9:22" x14ac:dyDescent="0.25">
@@ -31681,7 +31681,7 @@
         <v>0</v>
       </c>
       <c r="V984" s="14" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="985" spans="9:22" x14ac:dyDescent="0.25">
@@ -32274,7 +32274,7 @@
         <v>0</v>
       </c>
       <c r="V1008" s="14" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="1009" spans="4:22" x14ac:dyDescent="0.25">
@@ -32649,7 +32649,7 @@
         <v>82</v>
       </c>
       <c r="V1023" s="57" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="1024" spans="4:22" x14ac:dyDescent="0.25">
@@ -32829,7 +32829,7 @@
         <v>123</v>
       </c>
       <c r="D1030" s="48" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="H1030" s="47" t="s">
         <v>150</v>
@@ -32923,7 +32923,7 @@
     </row>
     <row r="1033" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D1033" s="48" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="H1033" s="47" t="s">
         <v>150</v>
@@ -33020,7 +33020,7 @@
         <v>82</v>
       </c>
       <c r="V1035" s="57" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="1036" spans="1:22" x14ac:dyDescent="0.25">
@@ -33098,7 +33098,7 @@
         <v>0</v>
       </c>
       <c r="V1038" s="14" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="1039" spans="1:22" x14ac:dyDescent="0.25">
@@ -33295,7 +33295,7 @@
         <v>0</v>
       </c>
       <c r="V1046" s="14" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="1047" spans="9:22" x14ac:dyDescent="0.25">
@@ -33324,7 +33324,7 @@
         <v>0</v>
       </c>
       <c r="V1047" s="14" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="1048" spans="9:22" x14ac:dyDescent="0.25">
@@ -33406,7 +33406,7 @@
         <v>0</v>
       </c>
       <c r="V1050" s="14" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="1051" spans="9:22" x14ac:dyDescent="0.25">
@@ -33508,7 +33508,7 @@
         <v>0</v>
       </c>
       <c r="V1054" s="14" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="1055" spans="9:22" x14ac:dyDescent="0.25">
@@ -33585,7 +33585,7 @@
         <v>82</v>
       </c>
       <c r="V1057" s="28" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="1058" spans="9:22" x14ac:dyDescent="0.25">
@@ -34371,7 +34371,7 @@
         <v>0</v>
       </c>
       <c r="V1088" s="14" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="1089" spans="9:22" x14ac:dyDescent="0.25">
@@ -34425,7 +34425,7 @@
         <v>0</v>
       </c>
       <c r="V1090" s="14" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="1091" spans="9:22" x14ac:dyDescent="0.25">
@@ -34454,7 +34454,7 @@
         <v>0</v>
       </c>
       <c r="V1091" s="14" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="1092" spans="9:22" x14ac:dyDescent="0.25">
@@ -34507,7 +34507,7 @@
         <v>0</v>
       </c>
       <c r="V1093" s="14" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="1094" spans="9:22" x14ac:dyDescent="0.25">
@@ -34584,7 +34584,7 @@
         <v>0</v>
       </c>
       <c r="V1096" s="14" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="1097" spans="9:22" x14ac:dyDescent="0.25">
@@ -34812,7 +34812,7 @@
     </row>
     <row r="1106" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F1106" s="54" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="G1106" s="47" t="s">
         <v>133</v>
@@ -34842,10 +34842,10 @@
     </row>
     <row r="1107" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B1107" s="54" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F1107" s="54" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="G1107" s="47" t="s">
         <v>133</v>
@@ -35019,7 +35019,7 @@
         <v>82</v>
       </c>
       <c r="V1113" s="28" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="1114" spans="1:22" x14ac:dyDescent="0.25">
@@ -35220,13 +35220,13 @@
         <v>64</v>
       </c>
       <c r="N1121" s="5" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="O1121" s="2" t="s">
         <v>0</v>
       </c>
       <c r="V1121" s="14" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="1122" spans="8:22" x14ac:dyDescent="0.25">
@@ -35328,7 +35328,7 @@
         <v>0</v>
       </c>
       <c r="V1125" s="14" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="1126" spans="8:22" x14ac:dyDescent="0.25">
@@ -35407,7 +35407,7 @@
         <v>0</v>
       </c>
       <c r="V1128" s="14" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="1129" spans="8:22" x14ac:dyDescent="0.25">
@@ -35768,7 +35768,7 @@
         <v>82</v>
       </c>
       <c r="V1142" s="33" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="1143" spans="9:22" x14ac:dyDescent="0.25">
@@ -35845,7 +35845,7 @@
         <v>0</v>
       </c>
       <c r="V1145" s="14" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="1146" spans="9:22" x14ac:dyDescent="0.25">
@@ -35972,7 +35972,7 @@
         <v>82</v>
       </c>
       <c r="V1150" s="8" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="1151" spans="9:22" x14ac:dyDescent="0.25">
@@ -36073,12 +36073,12 @@
         <v>82</v>
       </c>
       <c r="V1154" s="35" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="1155" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1155" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="E1155" s="47" t="s">
         <v>131</v>
@@ -36109,7 +36109,7 @@
     </row>
     <row r="1156" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1156" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="E1156" s="47" t="s">
         <v>131</v>
@@ -36146,7 +36146,7 @@
     </row>
     <row r="1157" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1157" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="H1157" s="47" t="s">
         <v>153</v>
@@ -36176,7 +36176,7 @@
     </row>
     <row r="1158" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1158" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="H1158" s="47" t="s">
         <v>153</v>
@@ -36209,7 +36209,7 @@
     </row>
     <row r="1159" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1159" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1159" s="8" t="s">
         <v>41</v>
@@ -36237,7 +36237,7 @@
     </row>
     <row r="1160" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1160" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1160" s="8" t="s">
         <v>41</v>
@@ -36264,7 +36264,7 @@
     </row>
     <row r="1161" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1161" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1161" s="8" t="s">
         <v>41</v>
@@ -36292,7 +36292,7 @@
     </row>
     <row r="1162" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1162" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1162" s="8" t="s">
         <v>41</v>
@@ -36319,7 +36319,7 @@
     </row>
     <row r="1163" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1163" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1163" s="8" t="s">
         <v>41</v>
@@ -36346,7 +36346,7 @@
     </row>
     <row r="1164" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1164" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1164" s="8" t="s">
         <v>41</v>
@@ -36373,7 +36373,7 @@
     </row>
     <row r="1165" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1165" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1165" s="8" t="s">
         <v>41</v>
@@ -36400,12 +36400,12 @@
         <v>82</v>
       </c>
       <c r="V1165" s="8" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="1166" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1166" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1166" s="8" t="s">
         <v>41</v>
@@ -36432,7 +36432,7 @@
     </row>
     <row r="1167" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1167" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1167" s="8" t="s">
         <v>41</v>
@@ -36459,7 +36459,7 @@
     </row>
     <row r="1168" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1168" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1168" s="8" t="s">
         <v>41</v>
@@ -36487,7 +36487,7 @@
     </row>
     <row r="1169" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1169" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1169" s="8" t="s">
         <v>41</v>
@@ -36514,7 +36514,7 @@
     </row>
     <row r="1170" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1170" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1170" s="8" t="s">
         <v>41</v>
@@ -36541,12 +36541,12 @@
         <v>0</v>
       </c>
       <c r="V1170" s="14" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="1171" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1171" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1171" s="8" t="s">
         <v>41</v>
@@ -36573,7 +36573,7 @@
     </row>
     <row r="1172" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1172" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1172" s="8" t="s">
         <v>41</v>
@@ -36600,7 +36600,7 @@
     </row>
     <row r="1173" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1173" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1173" s="8" t="s">
         <v>41</v>
@@ -36627,12 +36627,12 @@
         <v>0</v>
       </c>
       <c r="V1173" s="14" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="1174" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1174" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1174" s="8" t="s">
         <v>41</v>
@@ -36659,7 +36659,7 @@
     </row>
     <row r="1175" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1175" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1175" s="8" t="s">
         <v>41</v>
@@ -36686,7 +36686,7 @@
     </row>
     <row r="1176" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1176" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1176" s="8" t="s">
         <v>41</v>
@@ -36718,7 +36718,7 @@
     </row>
     <row r="1177" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1177" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1177" s="8" t="s">
         <v>41</v>
@@ -36748,7 +36748,7 @@
     </row>
     <row r="1178" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1178" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1178" s="8" t="s">
         <v>41</v>
@@ -36775,7 +36775,7 @@
     </row>
     <row r="1179" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1179" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1179" s="8" t="s">
         <v>41</v>
@@ -36802,7 +36802,7 @@
     </row>
     <row r="1180" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1180" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1180" s="8" t="s">
         <v>41</v>
@@ -36829,7 +36829,7 @@
     </row>
     <row r="1181" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1181" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1181" s="8" t="s">
         <v>41</v>
@@ -36856,7 +36856,7 @@
     </row>
     <row r="1182" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1182" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1182" s="8" t="s">
         <v>41</v>
@@ -36883,7 +36883,7 @@
     </row>
     <row r="1183" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1183" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1183" s="8" t="s">
         <v>41</v>
@@ -36910,12 +36910,12 @@
         <v>0</v>
       </c>
       <c r="V1183" s="14" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="1184" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1184" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1184" s="8" t="s">
         <v>41</v>
@@ -36942,12 +36942,12 @@
         <v>82</v>
       </c>
       <c r="V1184" s="35" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="1185" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1185" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1185" s="8" t="s">
         <v>41</v>
@@ -36974,7 +36974,7 @@
     </row>
     <row r="1186" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1186" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1186" s="8" t="s">
         <v>41</v>
@@ -37001,7 +37001,7 @@
     </row>
     <row r="1187" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1187" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1187" s="8" t="s">
         <v>41</v>
@@ -37028,7 +37028,7 @@
     </row>
     <row r="1188" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1188" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1188" s="8" t="s">
         <v>41</v>
@@ -37055,7 +37055,7 @@
     </row>
     <row r="1189" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1189" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1189" s="8" t="s">
         <v>41</v>
@@ -37082,12 +37082,12 @@
         <v>0</v>
       </c>
       <c r="V1189" s="14" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="1190" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1190" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1190" s="8" t="s">
         <v>41</v>
@@ -37114,7 +37114,7 @@
     </row>
     <row r="1191" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1191" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1191" s="8" t="s">
         <v>41</v>
@@ -37141,12 +37141,12 @@
         <v>82</v>
       </c>
       <c r="V1191" s="28" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="1192" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1192" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1192" s="8" t="s">
         <v>41</v>
@@ -37173,7 +37173,7 @@
     </row>
     <row r="1193" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1193" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1193" s="8" t="s">
         <v>41</v>
@@ -37200,7 +37200,7 @@
     </row>
     <row r="1194" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1194" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1194" s="8" t="s">
         <v>41</v>
@@ -37230,10 +37230,10 @@
     </row>
     <row r="1195" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1195" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="F1195" s="54" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1195" s="8" t="s">
         <v>41</v>
@@ -37257,7 +37257,7 @@
         <v>829</v>
       </c>
       <c r="S1195" s="41" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="T1195" s="2" t="s">
         <v>113</v>
@@ -37269,10 +37269,10 @@
         <v>123</v>
       </c>
       <c r="C1196" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="F1196" s="54" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I1196" s="8" t="s">
         <v>41</v>
@@ -37299,7 +37299,7 @@
     </row>
     <row r="1197" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1197" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1197" s="8" t="s">
         <v>41</v>
@@ -37326,12 +37326,12 @@
         <v>0</v>
       </c>
       <c r="V1197" s="14" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="1198" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1198" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1198" s="8" t="s">
         <v>41</v>
@@ -37358,7 +37358,7 @@
     </row>
     <row r="1199" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1199" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1199" s="8" t="s">
         <v>41</v>
@@ -37385,7 +37385,7 @@
     </row>
     <row r="1200" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1200" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1200" s="8" t="s">
         <v>41</v>
@@ -37412,7 +37412,7 @@
     </row>
     <row r="1201" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1201" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1201" s="8" t="s">
         <v>41</v>
@@ -37439,12 +37439,12 @@
         <v>82</v>
       </c>
       <c r="V1201" s="28" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="1202" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1202" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1202" s="8" t="s">
         <v>41</v>
@@ -37472,7 +37472,7 @@
     </row>
     <row r="1203" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1203" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I1203" s="8" t="s">
         <v>41</v>
@@ -37499,7 +37499,7 @@
     </row>
     <row r="1204" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1204" s="49" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="H1204" s="47" t="s">
         <v>154</v>
@@ -37529,7 +37529,7 @@
         <v>0</v>
       </c>
       <c r="V1204" s="14" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="1205" spans="3:22" x14ac:dyDescent="0.25">
@@ -37560,7 +37560,7 @@
         <v>0</v>
       </c>
       <c r="V1205" s="32" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="1206" spans="3:22" x14ac:dyDescent="0.25">
@@ -37695,7 +37695,7 @@
         <v>82</v>
       </c>
       <c r="V1210" s="8" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="1211" spans="3:22" x14ac:dyDescent="0.25">
@@ -37781,7 +37781,7 @@
         <v>0</v>
       </c>
       <c r="V1213" s="14" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="1214" spans="3:22" x14ac:dyDescent="0.25">
@@ -37935,7 +37935,7 @@
         <v>82</v>
       </c>
       <c r="V1219" s="8" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="1220" spans="4:22" x14ac:dyDescent="0.25">
@@ -38184,7 +38184,7 @@
         <v>0</v>
       </c>
       <c r="V1228" s="14" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="1229" spans="4:22" x14ac:dyDescent="0.25">
@@ -38468,7 +38468,7 @@
         <v>82</v>
       </c>
       <c r="V1239" s="14" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="1240" spans="8:22" x14ac:dyDescent="0.25">
@@ -38721,7 +38721,7 @@
         <v>15</v>
       </c>
       <c r="V1248" s="26" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="1249" spans="9:22" x14ac:dyDescent="0.25">
@@ -38833,7 +38833,7 @@
         <v>15</v>
       </c>
       <c r="V1252" s="28" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="1253" spans="9:22" x14ac:dyDescent="0.25">
@@ -38886,7 +38886,7 @@
         <v>0</v>
       </c>
       <c r="V1254" s="14" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="1255" spans="9:22" x14ac:dyDescent="0.25">
@@ -39043,7 +39043,7 @@
         <v>82</v>
       </c>
       <c r="V1260" s="31" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="1261" spans="9:22" x14ac:dyDescent="0.25">
@@ -39267,7 +39267,7 @@
         <v>82</v>
       </c>
       <c r="V1269" s="28" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="1270" spans="9:22" x14ac:dyDescent="0.25">
@@ -39346,7 +39346,7 @@
         <v>0</v>
       </c>
       <c r="V1272" s="14" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="1273" spans="9:22" x14ac:dyDescent="0.25">
@@ -39399,7 +39399,7 @@
         <v>0</v>
       </c>
       <c r="V1274" s="14" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="1275" spans="9:22" x14ac:dyDescent="0.25">
@@ -39428,7 +39428,7 @@
         <v>82</v>
       </c>
       <c r="V1275" s="35" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="1276" spans="9:22" x14ac:dyDescent="0.25">
@@ -39506,7 +39506,7 @@
         <v>82</v>
       </c>
       <c r="V1278" s="28" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="1279" spans="9:22" x14ac:dyDescent="0.25">
@@ -39754,7 +39754,7 @@
         <v>0</v>
       </c>
       <c r="V1287" s="14" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="1288" spans="1:22" x14ac:dyDescent="0.25">
@@ -39789,7 +39789,7 @@
         <v>82</v>
       </c>
       <c r="V1288" s="14" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="1289" spans="1:22" x14ac:dyDescent="0.25">
@@ -40029,7 +40029,7 @@
         <v>82</v>
       </c>
       <c r="V1297" s="28" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="1298" spans="8:22" x14ac:dyDescent="0.25">
@@ -40154,7 +40154,7 @@
         <v>0</v>
       </c>
       <c r="V1302" s="14" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="1303" spans="8:22" x14ac:dyDescent="0.25">
@@ -40210,7 +40210,7 @@
         <v>82</v>
       </c>
       <c r="V1304" s="35" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="1305" spans="8:22" x14ac:dyDescent="0.25">
@@ -40238,7 +40238,7 @@
         <v>15</v>
       </c>
       <c r="V1305" s="26" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="1306" spans="8:22" x14ac:dyDescent="0.25">
@@ -40267,7 +40267,7 @@
         <v>0</v>
       </c>
       <c r="V1306" s="14" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="1307" spans="8:22" x14ac:dyDescent="0.25">
@@ -40296,7 +40296,7 @@
         <v>82</v>
       </c>
       <c r="V1307" s="35" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="1308" spans="8:22" x14ac:dyDescent="0.25">
@@ -40397,7 +40397,7 @@
         <v>0</v>
       </c>
       <c r="V1311" s="14" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="1312" spans="8:22" x14ac:dyDescent="0.25">
@@ -40450,7 +40450,7 @@
         <v>0</v>
       </c>
       <c r="V1313" s="14" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="1314" spans="9:22" x14ac:dyDescent="0.25">
@@ -40556,7 +40556,7 @@
         <v>0</v>
       </c>
       <c r="V1317" s="14" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="1318" spans="9:22" x14ac:dyDescent="0.25">
@@ -40657,7 +40657,7 @@
         <v>0</v>
       </c>
       <c r="V1321" s="14" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="1322" spans="9:22" x14ac:dyDescent="0.25">
@@ -40686,7 +40686,7 @@
         <v>82</v>
       </c>
       <c r="V1322" s="31" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="1323" spans="9:22" x14ac:dyDescent="0.25">
@@ -40715,7 +40715,7 @@
         <v>89</v>
       </c>
       <c r="T1323" s="2" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="V1323" s="14"/>
     </row>
@@ -40869,7 +40869,7 @@
         <v>82</v>
       </c>
       <c r="V1329" s="28" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="1330" spans="4:22" x14ac:dyDescent="0.25">
@@ -40950,7 +40950,7 @@
         <v>0</v>
       </c>
       <c r="V1332" s="14" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="1333" spans="4:22" x14ac:dyDescent="0.25">
@@ -41024,7 +41024,7 @@
         <v>181</v>
       </c>
       <c r="N1335" s="55" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="O1335" s="1" t="s">
         <v>102</v>
@@ -41107,7 +41107,7 @@
         <v>82</v>
       </c>
       <c r="V1338" s="26" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="1339" spans="4:22" x14ac:dyDescent="0.25">
@@ -41145,7 +41145,7 @@
         <v>0</v>
       </c>
       <c r="V1339" s="14" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1340" spans="4:22" x14ac:dyDescent="0.25">
@@ -41258,7 +41258,7 @@
         <v>0</v>
       </c>
       <c r="V1343" s="14" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="1344" spans="4:22" x14ac:dyDescent="0.25">
@@ -41287,7 +41287,7 @@
         <v>0</v>
       </c>
       <c r="V1344" s="14" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="1345" spans="9:22" x14ac:dyDescent="0.25">
@@ -41316,7 +41316,7 @@
         <v>82</v>
       </c>
       <c r="V1345" s="28" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="1346" spans="9:22" x14ac:dyDescent="0.25">
@@ -41589,7 +41589,7 @@
         <v>82</v>
       </c>
       <c r="V1356" s="35" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="1357" spans="9:22" x14ac:dyDescent="0.25">
@@ -41667,7 +41667,7 @@
         <v>0</v>
       </c>
       <c r="V1359" s="14" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="1360" spans="9:22" x14ac:dyDescent="0.25">
@@ -41696,7 +41696,7 @@
         <v>0</v>
       </c>
       <c r="V1360" s="14" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="1361" spans="4:22" x14ac:dyDescent="0.25">
@@ -41728,7 +41728,7 @@
         <v>82</v>
       </c>
       <c r="V1361" s="14" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="1362" spans="4:22" x14ac:dyDescent="0.25">
@@ -41809,7 +41809,7 @@
         <v>82</v>
       </c>
       <c r="V1364" s="14" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="1365" spans="4:22" x14ac:dyDescent="0.25">
@@ -42054,7 +42054,7 @@
         <v>82</v>
       </c>
       <c r="V1373" s="14" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="1374" spans="4:22" x14ac:dyDescent="0.25">
@@ -42107,7 +42107,7 @@
         <v>0</v>
       </c>
       <c r="V1375" s="14" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="1376" spans="4:22" x14ac:dyDescent="0.25">
@@ -42142,7 +42142,7 @@
       <c r="T1376" s="43"/>
       <c r="U1376" s="43"/>
       <c r="V1376" s="14" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="1377" spans="8:22" x14ac:dyDescent="0.25">
@@ -42280,7 +42280,7 @@
         <v>82</v>
       </c>
       <c r="V1381" s="14" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="1382" spans="8:22" x14ac:dyDescent="0.25">
@@ -42456,7 +42456,7 @@
         <v>82</v>
       </c>
       <c r="V1388" s="28" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="1389" spans="8:22" x14ac:dyDescent="0.25">
@@ -42536,7 +42536,7 @@
         <v>82</v>
       </c>
       <c r="V1391" s="14" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="1392" spans="8:22" x14ac:dyDescent="0.25">
@@ -42690,7 +42690,7 @@
         <v>0</v>
       </c>
       <c r="V1397" s="14" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="1398" spans="9:22" x14ac:dyDescent="0.25">
@@ -42767,7 +42767,7 @@
         <v>82</v>
       </c>
       <c r="V1400" s="28" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1401" spans="9:22" x14ac:dyDescent="0.25">
@@ -42877,7 +42877,7 @@
         <v>0</v>
       </c>
       <c r="V1404" s="14" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="1405" spans="9:22" x14ac:dyDescent="0.25">
@@ -43004,7 +43004,7 @@
         <v>82</v>
       </c>
       <c r="V1409" s="14" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="1410" spans="9:22" x14ac:dyDescent="0.25">
@@ -43108,7 +43108,7 @@
         <v>0</v>
       </c>
       <c r="V1413" s="14" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="1414" spans="9:22" x14ac:dyDescent="0.25">
@@ -43232,7 +43232,7 @@
         <v>0</v>
       </c>
       <c r="V1418" s="8" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="1419" spans="9:22" x14ac:dyDescent="0.25">
@@ -43289,7 +43289,7 @@
         <v>95</v>
       </c>
       <c r="V1420" s="35" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="1421" spans="9:22" x14ac:dyDescent="0.25">
@@ -43415,7 +43415,7 @@
         <v>0</v>
       </c>
       <c r="V1425" s="14" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="1426" spans="8:22" x14ac:dyDescent="0.25">
@@ -43666,7 +43666,7 @@
         <v>0</v>
       </c>
       <c r="V1435" s="14" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="1436" spans="8:22" x14ac:dyDescent="0.25">
@@ -43698,7 +43698,7 @@
         <v>82</v>
       </c>
       <c r="V1436" s="28" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="1437" spans="8:22" x14ac:dyDescent="0.25">
@@ -43784,7 +43784,7 @@
         <v>0</v>
       </c>
       <c r="V1439" s="14" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="1440" spans="8:22" x14ac:dyDescent="0.25">
@@ -43813,7 +43813,7 @@
         <v>0</v>
       </c>
       <c r="V1440" s="14" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="1441" spans="1:22" x14ac:dyDescent="0.25">
@@ -43890,7 +43890,7 @@
         <v>0</v>
       </c>
       <c r="V1443" s="14" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="1444" spans="1:22" x14ac:dyDescent="0.25">
@@ -43943,7 +43943,7 @@
         <v>82</v>
       </c>
       <c r="V1445" s="32" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="1446" spans="1:22" x14ac:dyDescent="0.25">
@@ -44095,7 +44095,7 @@
         <v>0</v>
       </c>
       <c r="V1451" s="14" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="1452" spans="1:22" x14ac:dyDescent="0.25">
@@ -44124,7 +44124,7 @@
         <v>82</v>
       </c>
       <c r="V1452" s="28" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="1453" spans="1:22" x14ac:dyDescent="0.25">
@@ -44204,7 +44204,7 @@
     </row>
     <row r="1456" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1456" s="51" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="H1456" s="47" t="s">
         <v>160</v>
@@ -44237,7 +44237,7 @@
     </row>
     <row r="1457" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1457" s="51" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="H1457" s="47" t="s">
         <v>160</v>
@@ -44321,7 +44321,7 @@
         <v>82</v>
       </c>
       <c r="V1459" s="28" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="1460" spans="1:22" x14ac:dyDescent="0.25">
@@ -44401,7 +44401,7 @@
         <v>0</v>
       </c>
       <c r="V1462" s="14" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="1463" spans="1:22" x14ac:dyDescent="0.25">
@@ -44505,7 +44505,7 @@
         <v>82</v>
       </c>
       <c r="V1466" s="35" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="1467" spans="1:22" x14ac:dyDescent="0.25">
@@ -44684,7 +44684,7 @@
         <v>82</v>
       </c>
       <c r="V1473" s="14" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="1474" spans="6:22" x14ac:dyDescent="0.25">
@@ -44713,7 +44713,7 @@
         <v>0</v>
       </c>
       <c r="V1474" s="14" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="1475" spans="6:22" x14ac:dyDescent="0.25">
@@ -44742,7 +44742,7 @@
         <v>0</v>
       </c>
       <c r="V1475" s="14" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="1476" spans="6:22" x14ac:dyDescent="0.25">
@@ -44771,7 +44771,7 @@
         <v>0</v>
       </c>
       <c r="V1476" s="14" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="1477" spans="6:22" x14ac:dyDescent="0.25">
@@ -44800,7 +44800,7 @@
         <v>82</v>
       </c>
       <c r="V1477" s="8" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="1478" spans="6:22" x14ac:dyDescent="0.25">
@@ -44880,12 +44880,12 @@
         <v>95</v>
       </c>
       <c r="V1480" s="28" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="1481" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F1481" s="54" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="H1481" s="47" t="s">
         <v>161</v>
@@ -44915,7 +44915,7 @@
     </row>
     <row r="1482" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F1482" s="54" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="H1482" s="47" t="s">
         <v>161</v>
@@ -44972,7 +44972,7 @@
         <v>15</v>
       </c>
       <c r="V1483" s="26" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="1484" spans="6:22" x14ac:dyDescent="0.25">
@@ -45034,7 +45034,7 @@
         <v>0</v>
       </c>
       <c r="V1485" s="14" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1486" spans="6:22" x14ac:dyDescent="0.25">
@@ -45167,7 +45167,7 @@
         <v>82</v>
       </c>
       <c r="V1490" s="28" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="1491" spans="8:22" x14ac:dyDescent="0.25">
@@ -45268,7 +45268,7 @@
         <v>0</v>
       </c>
       <c r="V1494" s="60" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="1495" spans="8:22" x14ac:dyDescent="0.25">
@@ -45489,7 +45489,7 @@
         <v>122</v>
       </c>
       <c r="V1502" s="28" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="1503" spans="8:22" x14ac:dyDescent="0.25">
@@ -45713,7 +45713,7 @@
         <v>82</v>
       </c>
       <c r="V1511" s="35" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="1512" spans="5:22" x14ac:dyDescent="0.25">
@@ -45790,7 +45790,7 @@
         <v>82</v>
       </c>
       <c r="V1514" s="28" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="1515" spans="5:22" x14ac:dyDescent="0.25">
@@ -45819,7 +45819,7 @@
     </row>
     <row r="1516" spans="5:22" x14ac:dyDescent="0.25">
       <c r="F1516" s="54" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="I1516" s="8" t="s">
         <v>48</v>
@@ -45846,7 +45846,7 @@
     </row>
     <row r="1517" spans="5:22" x14ac:dyDescent="0.25">
       <c r="F1517" s="54" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="I1517" s="8" t="s">
         <v>48</v>
@@ -45873,7 +45873,7 @@
         <v>0</v>
       </c>
       <c r="V1517" s="14" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="1518" spans="5:22" x14ac:dyDescent="0.25">
@@ -45881,7 +45881,7 @@
         <v>131</v>
       </c>
       <c r="F1518" s="54" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="I1518" s="8" t="s">
         <v>48</v>
@@ -45911,7 +45911,7 @@
         <v>99</v>
       </c>
       <c r="V1518" s="26" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="1519" spans="5:22" x14ac:dyDescent="0.25">
@@ -45919,7 +45919,7 @@
         <v>131</v>
       </c>
       <c r="F1519" s="54" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="I1519" s="8" t="s">
         <v>48</v>
@@ -45973,7 +45973,7 @@
         <v>82</v>
       </c>
       <c r="V1520" s="14" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="1521" spans="1:22" x14ac:dyDescent="0.25">
@@ -46356,7 +46356,7 @@
         <v>82</v>
       </c>
       <c r="V1535" s="36" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="1536" spans="1:22" x14ac:dyDescent="0.25">
@@ -46586,7 +46586,7 @@
         <v>82</v>
       </c>
       <c r="V1544" s="28" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="1545" spans="8:22" x14ac:dyDescent="0.25">
@@ -46714,7 +46714,7 @@
         <v>82</v>
       </c>
       <c r="V1549" s="35" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="1550" spans="8:22" x14ac:dyDescent="0.25">
@@ -46773,7 +46773,7 @@
         <v>0</v>
       </c>
       <c r="V1551" s="14" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="1552" spans="8:22" x14ac:dyDescent="0.25">
@@ -46874,7 +46874,7 @@
         <v>82</v>
       </c>
       <c r="V1555" s="8" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="1556" spans="5:22" x14ac:dyDescent="0.25">
@@ -46954,7 +46954,7 @@
         <v>82</v>
       </c>
       <c r="V1558" s="14" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="1559" spans="5:22" x14ac:dyDescent="0.25">
@@ -47134,7 +47134,7 @@
         <v>82</v>
       </c>
       <c r="V1565" s="28" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="1566" spans="5:22" x14ac:dyDescent="0.25">
@@ -47215,7 +47215,7 @@
         <v>95</v>
       </c>
       <c r="V1568" s="32" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>